<commit_message>
products almost finished - companie's pages working
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\Documents\Work\FriFarma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roly\PycharmProjects\FriFarma\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$2:$I$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$I$51</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="230">
   <si>
     <t>Categoría</t>
   </si>
@@ -122,9 +122,6 @@
     <t>1g</t>
   </si>
   <si>
-    <t>Frasco ampolla x 1[i]</t>
-  </si>
-  <si>
     <t>Ceftazidima (inyectable)</t>
   </si>
   <si>
@@ -549,13 +546,184 @@
   </si>
   <si>
     <t>Penicilina con acción antipseudomonal con un inhibidor de las bectalactamasas.</t>
+  </si>
+  <si>
+    <t>Ciclofosfamida (Polvo para solución para infusión)</t>
+  </si>
+  <si>
+    <t>KUP</t>
+  </si>
+  <si>
+    <t>Ciclofosfamida como monohidrato</t>
+  </si>
+  <si>
+    <t>Frasco- vial</t>
+  </si>
+  <si>
+    <t>Citarabina</t>
+  </si>
+  <si>
+    <t>Citarabina (Solución inyectable)</t>
+  </si>
+  <si>
+    <t>100 mg/5mL y 500mg/10 mL</t>
+  </si>
+  <si>
+    <t>200 mg 1g</t>
+  </si>
+  <si>
+    <t>Gemcitabina (Polvo liofilizado para solución inyectable)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clorhidrato de Gemcitabina </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 200 mg y 1g y 2g</t>
+  </si>
+  <si>
+    <t>Metotrexato (Tableta)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metotrexato </t>
+  </si>
+  <si>
+    <t>2.5 mg</t>
+  </si>
+  <si>
+    <t>Blíster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dactinomicina </t>
+  </si>
+  <si>
+    <t>Dactinomicina (Liofilizado para Inyección)</t>
+  </si>
+  <si>
+    <t>0.5 mg</t>
+  </si>
+  <si>
+    <t>Idarubicina (Polvo liofilizado para solución inyectable)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Idarubicina HCL </t>
+  </si>
+  <si>
+    <t>5 mg</t>
+  </si>
+  <si>
+    <t>Alcaloides</t>
+  </si>
+  <si>
+    <t>Sulfato de Vinblastina (Polvo liofilizado para inyección)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sulfato de Vinblastina     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 mg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frasco- vial </t>
+  </si>
+  <si>
+    <t>Sulfato de Vincristina</t>
+  </si>
+  <si>
+    <t>Sulfato de Vincristina (Solución Inyectable)</t>
+  </si>
+  <si>
+    <t>1mg/mL</t>
+  </si>
+  <si>
+    <t>Dacarbazina</t>
+  </si>
+  <si>
+    <t>200 mg</t>
+  </si>
+  <si>
+    <t>Etoposido</t>
+  </si>
+  <si>
+    <t>100 mg/ 5 mL</t>
+  </si>
+  <si>
+    <t>Ampolla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hidroxiurea </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blíster </t>
+  </si>
+  <si>
+    <t>Leucovorina de Calcio</t>
+  </si>
+  <si>
+    <t>15mg/ 2mL Y 50 mg/ 5mL</t>
+  </si>
+  <si>
+    <t>Dacarbazina (Liofilizado para inyección)</t>
+  </si>
+  <si>
+    <t>Etopósido (Solución Inyectable)</t>
+  </si>
+  <si>
+    <t>Hidroxiurea (Cápsula)</t>
+  </si>
+  <si>
+    <t>Leucovorina de Calcio (Solución Inyectable)</t>
+  </si>
+  <si>
+    <t>Antianémicos</t>
+  </si>
+  <si>
+    <t>CIMAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eritropoyetina humana recombinante tipo alfa </t>
+  </si>
+  <si>
+    <t>Antianémico</t>
+  </si>
+  <si>
+    <t>2000 UI/mL</t>
+  </si>
+  <si>
+    <t>1mL/  Bulbo</t>
+  </si>
+  <si>
+    <t>Eritropoyetina humana recombinante tipo alfa</t>
+  </si>
+  <si>
+    <t>4000 UI/mL</t>
+  </si>
+  <si>
+    <t>Ior Epocim 2000 (Solución inyectable )</t>
+  </si>
+  <si>
+    <t>Ior Epocim 4000 (Solución inyectable )</t>
+  </si>
+  <si>
+    <t>Hematooncológicos</t>
+  </si>
+  <si>
+    <t>Ior Leukocim (Solución Inyectable)</t>
+  </si>
+  <si>
+    <t>Filgrastrim</t>
+  </si>
+  <si>
+    <t>Antineutropénico</t>
+  </si>
+  <si>
+    <t>30 MU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -571,13 +739,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -601,7 +781,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -618,7 +798,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -901,221 +1091,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S37"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="82.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="58.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="H3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>173</v>
+        <v>16</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>160</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>16</v>
+        <v>168</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>169</v>
+        <v>28</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>20</v>
@@ -1127,34 +1296,24 @@
         <v>6</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>32</v>
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>20</v>
@@ -1166,323 +1325,253 @@
         <v>6</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>127</v>
+        <v>35</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>9</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>10</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>160</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="H13" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>161</v>
+        <v>13</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>56</v>
+      <c r="F14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" t="s">
+        <v>64</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>62</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G15" t="s">
         <v>65</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>63</v>
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="G16" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" t="s">
         <v>47</v>
-      </c>
-      <c r="I16" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>69</v>
@@ -1491,7 +1580,7 @@
         <v>20</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>6</v>
@@ -1500,178 +1589,175 @@
         <v>73</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G18" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="I18" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>79</v>
+        <v>18</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G19" t="s">
-        <v>80</v>
+        <v>166</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>81</v>
+        <v>46</v>
       </c>
       <c r="I19" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>85</v>
+        <v>19</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="I20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G21" t="s">
-        <v>166</v>
+        <v>96</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="I21" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>93</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G22" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="I22" t="s">
-        <v>106</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G23" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="I23" t="s">
         <v>14</v>
@@ -1679,326 +1765,332 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>95</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="G24" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I24" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G25" t="s">
-        <v>104</v>
+        <v>161</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="I25" t="s">
-        <v>107</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G26" t="s">
         <v>162</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>113</v>
+        <v>46</v>
       </c>
       <c r="I26" t="s">
-        <v>158</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>114</v>
+        <v>26</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>116</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="G27" t="s">
         <v>163</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
       <c r="I27" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="G28" t="s">
         <v>164</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="I28" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>122</v>
+        <v>128</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>6</v>
+        <v>127</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G29" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="I29" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F30" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G30" t="s">
         <v>131</v>
       </c>
-      <c r="G30" t="s">
-        <v>132</v>
-      </c>
       <c r="H30" s="2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="I30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="G31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="I31" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="G32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="I32" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="G33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="I33" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>32</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>152</v>
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>151</v>
+        <v>60</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>153</v>
+        <v>66</v>
       </c>
       <c r="G34" t="s">
-        <v>132</v>
+        <v>65</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I34" t="s">
-        <v>155</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>63</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="G35" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>156</v>
@@ -2009,28 +2101,25 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>26</v>
+        <v>109</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>35</v>
+        <v>127</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="G36" t="s">
-        <v>36</v>
+        <v>161</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>157</v>
+        <v>112</v>
       </c>
       <c r="I36" t="s">
         <v>14</v>
@@ -2038,37 +2127,446 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>35</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>111</v>
+        <v>36</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>173</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>110</v>
+        <v>128</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="E37" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G37" t="s">
+        <v>131</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I37" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>178</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G37" t="s">
-        <v>162</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I37" t="s">
-        <v>14</v>
+      <c r="D38" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F38" t="s">
+        <v>177</v>
+      </c>
+      <c r="G38" t="s">
+        <v>131</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="I38" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
+        <v>38</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F39" t="s">
+        <v>182</v>
+      </c>
+      <c r="G39" t="s">
+        <v>131</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I39" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>184</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F40" t="s">
+        <v>185</v>
+      </c>
+      <c r="G40" t="s">
+        <v>131</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I40" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>189</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F41" t="s">
+        <v>188</v>
+      </c>
+      <c r="G41" t="s">
+        <v>131</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I41" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>191</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F42" t="s">
+        <v>192</v>
+      </c>
+      <c r="G42" t="s">
+        <v>131</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="I42" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>195</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F43" t="s">
+        <v>196</v>
+      </c>
+      <c r="G43" t="s">
+        <v>131</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="I43" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>200</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F44" t="s">
+        <v>199</v>
+      </c>
+      <c r="G44" t="s">
+        <v>131</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="I44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>44</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F45" t="s">
+        <v>202</v>
+      </c>
+      <c r="G45" t="s">
+        <v>131</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="I45" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>45</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F46" t="s">
+        <v>204</v>
+      </c>
+      <c r="G46" t="s">
+        <v>131</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I46" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>213</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F47" t="s">
+        <v>207</v>
+      </c>
+      <c r="G47" t="s">
+        <v>131</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I47" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>47</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F48" t="s">
+        <v>209</v>
+      </c>
+      <c r="G48" t="s">
+        <v>131</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="I48" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>223</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F49" t="s">
+        <v>217</v>
+      </c>
+      <c r="G49" t="s">
+        <v>218</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="I49" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>224</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F50" t="s">
+        <v>221</v>
+      </c>
+      <c r="G50" t="s">
+        <v>218</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I50" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>226</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F51" t="s">
+        <v>227</v>
+      </c>
+      <c r="G51" t="s">
+        <v>228</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="I51" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I37">
-    <sortState ref="A3:I37">
-      <sortCondition ref="A2:A37"/>
+  <autoFilter ref="A1:I51">
+    <sortState ref="A2:I51">
+      <sortCondition ref="A1:A51"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>